<commit_message>
Modificaciones para medida de Datos
</commit_message>
<xml_diff>
--- a/PracticaGestionDatos/resources/stats bdd.xlsx
+++ b/PracticaGestionDatos/resources/stats bdd.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laura\Universidad\Curso 3º\Gestion de datos\GDD_KL\PracticaGestionDatos\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Laura\Universidad\Gestion de datos\Practica1\GDD_KL\PracticaGestionDatos\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8148" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>XML</t>
   </si>
@@ -37,14 +38,23 @@
   <si>
     <t>Iteraciones</t>
   </si>
+  <si>
+    <t>1 Partida</t>
+  </si>
+  <si>
+    <t>2 Partidas</t>
+  </si>
+  <si>
+    <t>3 Partidas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -81,16 +91,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,7 +424,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -416,11 +432,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="458545792"/>
-        <c:axId val="458548536"/>
+        <c:axId val="378566560"/>
+        <c:axId val="377578320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="458545792"/>
+        <c:axId val="378566560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,7 +462,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-ES"/>
-                  <a:t>Número de iteraciones</a:t>
+                  <a:t>Número de MOVIMIENTOS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -523,7 +539,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458548536"/>
+        <c:crossAx val="377578320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -531,7 +547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="458548536"/>
+        <c:axId val="377578320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +651,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="458545792"/>
+        <c:crossAx val="378566560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1092,11 +1108,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="580156400"/>
-        <c:axId val="580162672"/>
+        <c:axId val="375690096"/>
+        <c:axId val="155597160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="580156400"/>
+        <c:axId val="375690096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1138,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-ES"/>
-                  <a:t>Número de iteraciones</a:t>
+                  <a:t>Número de MOVIMIENTOS</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1199,7 +1215,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580162672"/>
+        <c:crossAx val="155597160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1207,7 +1223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="580162672"/>
+        <c:axId val="155597160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,7 +1327,1715 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580156400"/>
+        <c:crossAx val="375690096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Memoria consumida con 1 partida guardada</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>XML</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$25:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>663</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2546</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3117</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3729</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mongo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>719</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1869</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2799</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4959</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="532680632"/>
+        <c:axId val="532682200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="532680632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Número de movimientos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532682200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="532682200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Memoria (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532680632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="40000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </a:rPr>
+              <a:t>Memoria consumida con 2 partidas guardadas</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>XML</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$14:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$B$14:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>876</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3521</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4670</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5820</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mongo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$14:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$C$14:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1195</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4415</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5355</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9675</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="403280368"/>
+        <c:axId val="403281544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="403280368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Número de movimientos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403281544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="403281544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Memoria (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403280368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="40000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </a:rPr>
+              <a:t>Memoria consumida con 3 partidas guardadas</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>XML</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$14:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$B$25:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2402</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5061</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6815</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8509</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10311</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17971</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mongo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Hoja2!$A$14:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$C$25:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1671</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3741</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7911</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14391</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="405102488"/>
+        <c:axId val="540221432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="405102488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Número de movimientos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="540221432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="540221432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-ES"/>
+                  <a:t>Memoria (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="405102488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1482,6 +3206,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -1979,6 +3823,1494 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2533,6 +5865,103 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>777240</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3058,16 +6487,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3093,7 +6522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>5</v>
       </c>
@@ -3119,7 +6548,7 @@
         <v>1.2430000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>20</v>
       </c>
@@ -3145,7 +6574,7 @@
         <v>1.163</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>50</v>
       </c>
@@ -3171,7 +6600,7 @@
         <v>1.603</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>70</v>
       </c>
@@ -3197,7 +6626,7 @@
         <v>1.3380000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>90</v>
       </c>
@@ -3223,7 +6652,7 @@
         <v>1.147</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>110</v>
       </c>
@@ -3249,7 +6678,7 @@
         <v>1.2190000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>200</v>
       </c>
@@ -3280,4 +6709,395 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>663</v>
+      </c>
+      <c r="C3" s="3">
+        <v>379</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1099</v>
+      </c>
+      <c r="C4" s="3">
+        <v>719</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1987</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1409</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2546</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1869</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>90</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3117</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2329</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>110</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3729</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2799</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>200</v>
+      </c>
+      <c r="B9" s="3">
+        <v>6265</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4959</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3">
+        <v>876</v>
+      </c>
+      <c r="C14" s="3">
+        <v>515</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1748</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1195</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3521</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2575</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>70</v>
+      </c>
+      <c r="B17" s="3">
+        <v>4670</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3495</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>90</v>
+      </c>
+      <c r="B18" s="3">
+        <v>5820</v>
+      </c>
+      <c r="C18" s="3">
+        <v>4415</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>110</v>
+      </c>
+      <c r="B19" s="3">
+        <v>7011</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5355</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>200</v>
+      </c>
+      <c r="B20" s="3">
+        <v>12097</v>
+      </c>
+      <c r="C20" s="3">
+        <v>9675</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1096</v>
+      </c>
+      <c r="C25" s="3">
+        <v>651</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2402</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1671</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>50</v>
+      </c>
+      <c r="B27" s="3">
+        <v>5061</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3741</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>70</v>
+      </c>
+      <c r="B28" s="3">
+        <v>6815</v>
+      </c>
+      <c r="C28" s="3">
+        <v>5121</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>90</v>
+      </c>
+      <c r="B29" s="3">
+        <v>8509</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6501</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>110</v>
+      </c>
+      <c r="B30" s="3">
+        <v>10311</v>
+      </c>
+      <c r="C30" s="3">
+        <v>7911</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>200</v>
+      </c>
+      <c r="B31" s="3">
+        <v>17971</v>
+      </c>
+      <c r="C31" s="3">
+        <v>14391</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>